<commit_message>
work on gum seed data
all existing are uploading correctly now
</commit_message>
<xml_diff>
--- a/db/gums seed data v6.xlsx
+++ b/db/gums seed data v6.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="0" windowWidth="25400" windowHeight="19260" tabRatio="500"/>
+    <workbookView xWindow="3040" yWindow="0" windowWidth="27820" windowHeight="19260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Working Data" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2049" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2050" uniqueCount="906">
   <si>
     <t>Cool Mint + Melon Fresco</t>
   </si>
@@ -3527,7 +3527,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3573,6 +3573,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="673">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4579,8 +4582,8 @@
   <dimension ref="A1:N311"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M177" sqref="M177"/>
+      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B165" sqref="B165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6644,10 +6647,10 @@
       </c>
       <c r="M46" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>dentyne_ice_peppermint.png</v>
+        <v>dentyne_ice_peppermint.jpg</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="47" spans="1:14" s="9" customFormat="1">
@@ -6728,10 +6731,10 @@
       </c>
       <c r="M48" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>dentyne_ice_arctic_chill.png</v>
+        <v>dentyne_ice_arctic_chill.jpg</v>
       </c>
       <c r="N48" s="4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="49" spans="1:14">
@@ -6770,14 +6773,14 @@
       </c>
       <c r="M49" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>dentyne_ice_mint_frost.png</v>
+        <v>dentyne_ice_mint_frost.jpg</v>
       </c>
       <c r="N49" s="4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="50" spans="1:14">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="9" t="s">
         <v>813</v>
       </c>
       <c r="B50" s="7" t="s">
@@ -6812,14 +6815,14 @@
       </c>
       <c r="M50" s="4" t="str">
         <f t="shared" ref="M50" si="4">CONCATENATE(A50,".",N50)</f>
-        <v>dentyne_ice_mint_medley.png</v>
+        <v>dentyne_ice_mint_medley.jpg</v>
       </c>
       <c r="N50" s="4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="51" spans="1:14">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="9" t="s">
         <v>818</v>
       </c>
       <c r="B51" s="7" t="s">
@@ -6854,14 +6857,14 @@
       </c>
       <c r="M51" s="4" t="str">
         <f t="shared" ref="M51" si="5">CONCATENATE(A51,".",N51)</f>
-        <v>dentyne_ice_shiver_mint.png</v>
+        <v>dentyne_ice_shiver_mint.jpg</v>
       </c>
       <c r="N51" s="4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="52" spans="1:14">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="9" t="s">
         <v>824</v>
       </c>
       <c r="B52" s="7" t="s">
@@ -6896,10 +6899,10 @@
       </c>
       <c r="M52" s="4" t="str">
         <f t="shared" ref="M52" si="6">CONCATENATE(A52,".",N52)</f>
-        <v>dentyne_ice_vanilla_chill.png</v>
+        <v>dentyne_ice_vanilla_chill.jpg</v>
       </c>
       <c r="N52" s="4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="53" spans="1:14">
@@ -7888,7 +7891,7 @@
         <v>156</v>
       </c>
       <c r="D76" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E76" s="4">
         <v>0</v>
@@ -7930,7 +7933,7 @@
         <v>566</v>
       </c>
       <c r="D77" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" s="4">
         <v>0</v>
@@ -7972,7 +7975,7 @@
         <v>156</v>
       </c>
       <c r="D78" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E78" s="4">
         <v>0</v>
@@ -8014,7 +8017,7 @@
         <v>156</v>
       </c>
       <c r="D79" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79" s="4">
         <v>0</v>
@@ -8056,7 +8059,7 @@
         <v>156</v>
       </c>
       <c r="D80" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80" s="4">
         <v>0</v>
@@ -8098,7 +8101,7 @@
         <v>156</v>
       </c>
       <c r="D81" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81" s="4">
         <v>0</v>
@@ -8140,7 +8143,7 @@
         <v>156</v>
       </c>
       <c r="D82" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E82" s="4">
         <v>0</v>
@@ -8182,7 +8185,7 @@
         <v>156</v>
       </c>
       <c r="D83" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83" s="4">
         <v>0</v>
@@ -8840,10 +8843,10 @@
       </c>
       <c r="M98" s="4" t="str">
         <f t="shared" ref="M98" si="9">CONCATENATE(A98,".",N98)</f>
-        <v>extra_fruit_sensations_strawberry_banana.png</v>
+        <v>extra_fruit_sensations_strawberry_banana.jpg</v>
       </c>
       <c r="N98" s="4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="99" spans="1:14">
@@ -9515,10 +9518,10 @@
       </c>
       <c r="M114" s="4" t="str">
         <f t="shared" si="7"/>
-        <v>5_gum_swerve.jpg</v>
+        <v>5_gum_swerve.jpeg</v>
       </c>
       <c r="N114" s="4" t="s">
-        <v>543</v>
+        <v>651</v>
       </c>
     </row>
     <row r="115" spans="1:14">
@@ -9683,10 +9686,10 @@
       </c>
       <c r="M118" s="4" t="str">
         <f t="shared" ref="M118" si="11">CONCATENATE(A118,".",N118)</f>
-        <v>5_gum_lush.png</v>
+        <v>5_gum_lush.jpg</v>
       </c>
       <c r="N118" s="4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="119" spans="1:14">
@@ -9722,11 +9725,11 @@
         <v>0</v>
       </c>
       <c r="M119" s="4" t="str">
-        <f t="shared" ref="M119" si="12">CONCATENATE(A119,".",N119)</f>
-        <v>5_gum_zing.png</v>
+        <f t="shared" ref="M119:M121" si="12">CONCATENATE(A119,".",N119)</f>
+        <v>5_gum_zing.jpg</v>
       </c>
       <c r="N119" s="4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="120" spans="1:14">
@@ -9760,8 +9763,9 @@
       <c r="L120" s="4">
         <v>0</v>
       </c>
-      <c r="M120" s="4" t="s">
-        <v>522</v>
+      <c r="M120" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>wrigleys_winterfresh.png</v>
       </c>
       <c r="N120" s="4" t="s">
         <v>542</v>
@@ -9798,8 +9802,9 @@
       <c r="L121" s="4">
         <v>0</v>
       </c>
-      <c r="M121" s="4" t="s">
-        <v>523</v>
+      <c r="M121" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>wrigleys_spearmint.jpg</v>
       </c>
       <c r="N121" s="4" t="s">
         <v>543</v>
@@ -11276,7 +11281,7 @@
       </c>
     </row>
     <row r="159" spans="1:14">
-      <c r="A159" s="13" t="s">
+      <c r="A159" s="9" t="s">
         <v>514</v>
       </c>
       <c r="B159" s="7" t="s">
@@ -11311,14 +11316,14 @@
       </c>
       <c r="M159" s="4" t="str">
         <f t="shared" si="14"/>
-        <v>orbit_mist_raspberry_lemon_dew.png</v>
+        <v>orbit_mist_raspberry_lemon_dew.jpg</v>
       </c>
       <c r="N159" s="4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="160" spans="1:14">
-      <c r="A160" s="13" t="s">
+      <c r="A160" s="9" t="s">
         <v>515</v>
       </c>
       <c r="B160" s="7" t="s">
@@ -11353,14 +11358,14 @@
       </c>
       <c r="M160" s="4" t="str">
         <f t="shared" si="14"/>
-        <v>orbit_mist_peppermint_spray.png</v>
+        <v>orbit_mist_peppermint_spray.jpg</v>
       </c>
       <c r="N160" s="4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="161" spans="1:14">
-      <c r="A161" s="13" t="s">
+      <c r="A161" s="9" t="s">
         <v>516</v>
       </c>
       <c r="B161" s="7" t="s">
@@ -11395,14 +11400,14 @@
       </c>
       <c r="M161" s="4" t="str">
         <f t="shared" si="14"/>
-        <v>orbit_mist_spearmint_spritzer.png</v>
+        <v>orbit_mist_spearmint_spritzer.jpg</v>
       </c>
       <c r="N161" s="4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="162" spans="1:14">
-      <c r="A162" s="13" t="s">
+      <c r="A162" s="9" t="s">
         <v>517</v>
       </c>
       <c r="B162" s="7" t="s">
@@ -11437,14 +11442,14 @@
       </c>
       <c r="M162" s="4" t="str">
         <f t="shared" si="14"/>
-        <v>orbit_mist_watermelon_spring.png</v>
+        <v>orbit_mist_watermelon_spring.jpg</v>
       </c>
       <c r="N162" s="4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="163" spans="1:14">
-      <c r="A163" s="13" t="s">
+      <c r="A163" s="9" t="s">
         <v>518</v>
       </c>
       <c r="B163" s="7" t="s">
@@ -11479,10 +11484,10 @@
       </c>
       <c r="M163" s="4" t="str">
         <f t="shared" si="14"/>
-        <v>orbit_mist_crisp_mint_waterfall.png</v>
+        <v>orbit_mist_crisp_mint_waterfall.jpg</v>
       </c>
       <c r="N163" s="4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="164" spans="1:14">
@@ -12026,7 +12031,7 @@
       <c r="A177" s="4" t="s">
         <v>698</v>
       </c>
-      <c r="B177" s="7" t="s">
+      <c r="B177" s="21" t="s">
         <v>643</v>
       </c>
       <c r="C177" s="7" t="s">
@@ -12043,13 +12048,19 @@
       </c>
       <c r="H177" s="4" t="s">
         <v>625</v>
+      </c>
+      <c r="K177" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L177" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:12">
       <c r="A178" s="4" t="s">
         <v>699</v>
       </c>
-      <c r="B178" s="7" t="s">
+      <c r="B178" s="21" t="s">
         <v>644</v>
       </c>
       <c r="C178" s="7" t="s">
@@ -12066,13 +12077,19 @@
       </c>
       <c r="H178" s="4" t="s">
         <v>628</v>
+      </c>
+      <c r="K178" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L178" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:12">
       <c r="A179" s="4" t="s">
         <v>700</v>
       </c>
-      <c r="B179" s="7" t="s">
+      <c r="B179" s="21" t="s">
         <v>645</v>
       </c>
       <c r="C179" s="7" t="s">
@@ -12089,13 +12106,19 @@
       </c>
       <c r="H179" s="4" t="s">
         <v>630</v>
+      </c>
+      <c r="K179" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L179" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="1:12">
       <c r="A180" s="4" t="s">
         <v>701</v>
       </c>
-      <c r="B180" s="7" t="str">
+      <c r="B180" s="21" t="str">
         <f t="shared" ref="B180:B187" si="17">CONCATENATE(G180," ",H180)</f>
         <v>ICE BREAKERS (R) Ice Cubes (R) Peppermint</v>
       </c>
@@ -12129,7 +12152,7 @@
       <c r="A181" s="4" t="s">
         <v>702</v>
       </c>
-      <c r="B181" s="7" t="str">
+      <c r="B181" s="21" t="str">
         <f t="shared" si="17"/>
         <v>ICE BREAKERS (R) Ice Cubes (R) Spearmint</v>
       </c>
@@ -12163,7 +12186,7 @@
       <c r="A182" s="4" t="s">
         <v>703</v>
       </c>
-      <c r="B182" s="7" t="str">
+      <c r="B182" s="21" t="str">
         <f t="shared" si="17"/>
         <v>ICE BREAKERS (R) Ice Cubes (R) Rasberry Sorbet</v>
       </c>
@@ -12196,7 +12219,7 @@
       <c r="A183" s="4" t="s">
         <v>704</v>
       </c>
-      <c r="B183" s="7" t="str">
+      <c r="B183" s="21" t="str">
         <f t="shared" si="17"/>
         <v>ICE BREAKERS (R) Ice Cubes (R) Kiwi Watermelon </v>
       </c>
@@ -12229,7 +12252,7 @@
       <c r="A184" s="4" t="s">
         <v>705</v>
       </c>
-      <c r="B184" s="7" t="str">
+      <c r="B184" s="21" t="str">
         <f t="shared" si="17"/>
         <v>ICE BREAKERS (R) Ice Cubes (R) Strawberry Smoothie Gum</v>
       </c>
@@ -12262,7 +12285,7 @@
       <c r="A185" s="4" t="s">
         <v>706</v>
       </c>
-      <c r="B185" s="7" t="str">
+      <c r="B185" s="21" t="str">
         <f t="shared" si="17"/>
         <v>ICE BREAKERS (R) Ice Cubes (R) Wintergreen</v>
       </c>
@@ -12295,7 +12318,7 @@
       <c r="A186" s="4" t="s">
         <v>707</v>
       </c>
-      <c r="B186" s="7" t="str">
+      <c r="B186" s="21" t="str">
         <f t="shared" si="17"/>
         <v>ICE BREAKERS (R) Ice Cubes (R) Cool Lemon (R)</v>
       </c>
@@ -12328,7 +12351,7 @@
       <c r="A187" s="4" t="s">
         <v>708</v>
       </c>
-      <c r="B187" s="7" t="str">
+      <c r="B187" s="21" t="str">
         <f t="shared" si="17"/>
         <v>ICE BREAKERS (R) Ice Cubes (R) Bubble Breeze (R)</v>
       </c>
@@ -12361,7 +12384,7 @@
       <c r="A188" s="4" t="s">
         <v>726</v>
       </c>
-      <c r="B188" s="7" t="str">
+      <c r="B188" s="21" t="str">
         <f t="shared" ref="B188" si="18">CONCATENATE(G188," ",H188)</f>
         <v>ICE BREAKERS (R) Ice Cubes (R) White Mango Kiwi Cooler</v>
       </c>
@@ -12385,7 +12408,7 @@
       <c r="A189" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="B189" s="7" t="str">
+      <c r="B189" s="21" t="str">
         <f t="shared" ref="B189:B195" si="19">CONCATENATE(G189," ",H189)</f>
         <v>ICE BREAKERS (R) Ice Cubes (R) White Winter Green Splash</v>
       </c>
@@ -12409,7 +12432,7 @@
       <c r="A190" s="4" t="s">
         <v>741</v>
       </c>
-      <c r="B190" s="7" t="str">
+      <c r="B190" s="21" t="str">
         <f t="shared" ref="B190:B191" si="20">CONCATENATE(G190," ",H190)</f>
         <v>ICE BREAKERS (R) Stick Gum Coolmint</v>
       </c>
@@ -12433,7 +12456,7 @@
       <c r="A191" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="B191" s="7" t="str">
+      <c r="B191" s="21" t="str">
         <f t="shared" si="20"/>
         <v>ICE BREAKERS (R) Stick Gum Wintergreen</v>
       </c>
@@ -13233,10 +13256,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A133"/>
+  <dimension ref="A1:A210"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A20" workbookViewId="0">
-      <selection sqref="A1:A49"/>
+    <sheetView showRuler="0" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="A158" sqref="A158:A175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13511,7 +13534,7 @@
     <row r="45" spans="1:1">
       <c r="A45" t="str">
         <f>CONCATENATE('Working Data'!A46,"|",'Working Data'!B46,"|",'Working Data'!C46,"|",'Working Data'!D46,"|",'Working Data'!E46,"|",'Working Data'!F46,"|",'Working Data'!G46,"|",'Working Data'!H46,"|",'Working Data'!I46,"|",'Working Data'!J46,"|",'Working Data'!K46,"|",'Working Data'!L46,"|",'Working Data'!M46)</f>
-        <v>dentyne_ice_peppermint|Dentyne Ice Peppermint|012546312554|1|0|Mondelez International Kraft Foods Cadbury|Dentyne Ice|Peppermint|Stay on top of your game with a flavor that's classic and timeless.||United States|0|dentyne_ice_peppermint.png</v>
+        <v>dentyne_ice_peppermint|Dentyne Ice Peppermint|012546312554|1|0|Mondelez International Kraft Foods Cadbury|Dentyne Ice|Peppermint|Stay on top of your game with a flavor that's classic and timeless.||United States|0|dentyne_ice_peppermint.jpg</v>
       </c>
     </row>
     <row r="46" spans="1:1">
@@ -13523,31 +13546,31 @@
     <row r="47" spans="1:1">
       <c r="A47" t="str">
         <f>CONCATENATE('Working Data'!A48,"|",'Working Data'!B48,"|",'Working Data'!C48,"|",'Working Data'!D48,"|",'Working Data'!E48,"|",'Working Data'!F48,"|",'Working Data'!G48,"|",'Working Data'!H48,"|",'Working Data'!I48,"|",'Working Data'!J48,"|",'Working Data'!K48,"|",'Working Data'!L48,"|",'Working Data'!M48)</f>
-        <v>dentyne_ice_arctic_chill|Dentyne Ice Arctic Chill|012546312417 012546300599 012546310512|1|0|Mondelez International Kraft Foods Cadbury|Dentyne Ice|Arctic Chill|Before introducing yourself, get intense freshness from a bold, icy flavor.||United States|0|dentyne_ice_arctic_chill.png</v>
+        <v>dentyne_ice_arctic_chill|Dentyne Ice Arctic Chill|012546312417 012546300599 012546310512|1|0|Mondelez International Kraft Foods Cadbury|Dentyne Ice|Arctic Chill|Before introducing yourself, get intense freshness from a bold, icy flavor.||United States|0|dentyne_ice_arctic_chill.jpg</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="str">
         <f>CONCATENATE('Working Data'!A49,"|",'Working Data'!B49,"|",'Working Data'!C49,"|",'Working Data'!D49,"|",'Working Data'!E49,"|",'Working Data'!F49,"|",'Working Data'!G49,"|",'Working Data'!H49,"|",'Working Data'!I49,"|",'Working Data'!J49,"|",'Working Data'!K49,"|",'Working Data'!L49,"|",'Working Data'!M49)</f>
-        <v>dentyne_ice_mint_frost|Dentyne Ice Mint Frost|0|1|0|Mondelez International Kraft Foods Cadbury|Dentyne Ice|Mint Frost|Be ready for anything with a refreshing hint of cool, frosty mint.||United States|0|dentyne_ice_mint_frost.png</v>
+        <v>dentyne_ice_mint_frost|Dentyne Ice Mint Frost|0|1|0|Mondelez International Kraft Foods Cadbury|Dentyne Ice|Mint Frost|Be ready for anything with a refreshing hint of cool, frosty mint.||United States|0|dentyne_ice_mint_frost.jpg</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="str">
         <f>CONCATENATE('Working Data'!A50,"|",'Working Data'!B50,"|",'Working Data'!C50,"|",'Working Data'!D50,"|",'Working Data'!E50,"|",'Working Data'!F50,"|",'Working Data'!G50,"|",'Working Data'!H50,"|",'Working Data'!I50,"|",'Working Data'!J50,"|",'Working Data'!K50,"|",'Working Data'!L50,"|",'Working Data'!M50)</f>
-        <v>dentyne_ice_mint_medley|Dentyne Ice Mint Medley|012546312097|1|0|Mondelez International Kraft Foods Cadbury|Dentyne Ice|Mint Medley|Be ready for anything with a refreshing hint of cool, frosty mint.||United States|0|dentyne_ice_mint_medley.png</v>
+        <v>dentyne_ice_mint_medley|Dentyne Ice Mint Medley|012546312097|1|0|Mondelez International Kraft Foods Cadbury|Dentyne Ice|Mint Medley|Be ready for anything with a refreshing hint of cool, frosty mint.||United States|0|dentyne_ice_mint_medley.jpg</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="str">
         <f>CONCATENATE('Working Data'!A51,"|",'Working Data'!B51,"|",'Working Data'!C51,"|",'Working Data'!D51,"|",'Working Data'!E51,"|",'Working Data'!F51,"|",'Working Data'!G51,"|",'Working Data'!H51,"|",'Working Data'!I51,"|",'Working Data'!J51,"|",'Working Data'!K51,"|",'Working Data'!L51,"|",'Working Data'!M51)</f>
-        <v>dentyne_ice_shiver_mint|Dentyne Ice Shiver Mint|012546300094|1|0|Mondelez International Kraft Foods Cadbury|Dentyne Ice|Shiver Mint|Be ready for anything with a refreshing hint of cool, frosty mint.||United States|0|dentyne_ice_shiver_mint.png</v>
+        <v>dentyne_ice_shiver_mint|Dentyne Ice Shiver Mint|012546300094|1|0|Mondelez International Kraft Foods Cadbury|Dentyne Ice|Shiver Mint|Be ready for anything with a refreshing hint of cool, frosty mint.||United States|0|dentyne_ice_shiver_mint.jpg</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="str">
         <f>CONCATENATE('Working Data'!A52,"|",'Working Data'!B52,"|",'Working Data'!C52,"|",'Working Data'!D52,"|",'Working Data'!E52,"|",'Working Data'!F52,"|",'Working Data'!G52,"|",'Working Data'!H52,"|",'Working Data'!I52,"|",'Working Data'!J52,"|",'Working Data'!K52,"|",'Working Data'!L52,"|",'Working Data'!M52)</f>
-        <v>dentyne_ice_vanilla_chill|Dentyne Ice Vanilla Chill|012546302814|1|0|Mondelez International Kraft Foods Cadbury|Dentyne Ice|Vanilla Chill|Be ready for anything with a refreshing hint of cool, frosty mint.||United States|0|dentyne_ice_vanilla_chill.png</v>
+        <v>dentyne_ice_vanilla_chill|Dentyne Ice Vanilla Chill|012546302814|1|0|Mondelez International Kraft Foods Cadbury|Dentyne Ice|Vanilla Chill|Be ready for anything with a refreshing hint of cool, frosty mint.||United States|0|dentyne_ice_vanilla_chill.jpg</v>
       </c>
     </row>
     <row r="52" spans="1:1">
@@ -13691,49 +13714,49 @@
     <row r="75" spans="1:1">
       <c r="A75" t="str">
         <f>CONCATENATE('Working Data'!A76,"|",'Working Data'!B76,"|",'Working Data'!C76,"|",'Working Data'!D76,"|",'Working Data'!E76,"|",'Working Data'!F76,"|",'Working Data'!G76,"|",'Working Data'!H76,"|",'Working Data'!I76,"|",'Working Data'!J76,"|",'Working Data'!K76,"|",'Working Data'!L76,"|",'Working Data'!M76)</f>
-        <v>stride_nonstop_mint|Stride Nonstop Mint|0|0|0|Mondelez International Kraft Foods Cadbury|Stride|Nonstop Mint|?||United States|0|stride_nonstop_mint.jpg</v>
+        <v>stride_nonstop_mint|Stride Nonstop Mint|0|1|0|Mondelez International Kraft Foods Cadbury|Stride|Nonstop Mint|?||United States|0|stride_nonstop_mint.jpg</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="str">
         <f>CONCATENATE('Working Data'!A77,"|",'Working Data'!B77,"|",'Working Data'!C77,"|",'Working Data'!D77,"|",'Working Data'!E77,"|",'Working Data'!F77,"|",'Working Data'!G77,"|",'Working Data'!H77,"|",'Working Data'!I77,"|",'Working Data'!J77,"|",'Working Data'!K77,"|",'Working Data'!L77,"|",'Working Data'!M77)</f>
-        <v>stride_winterblue|Stride Winterblue|012546680028|0|0|Mondelez International Kraft Foods Cadbury|Stride|Winterblue|?||United States|0|stride_winterblue.jpg</v>
+        <v>stride_winterblue|Stride Winterblue|012546680028|1|0|Mondelez International Kraft Foods Cadbury|Stride|Winterblue|?||United States|0|stride_winterblue.jpg</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="str">
         <f>CONCATENATE('Working Data'!A78,"|",'Working Data'!B78,"|",'Working Data'!C78,"|",'Working Data'!D78,"|",'Working Data'!E78,"|",'Working Data'!F78,"|",'Working Data'!G78,"|",'Working Data'!H78,"|",'Working Data'!I78,"|",'Working Data'!J78,"|",'Working Data'!K78,"|",'Working Data'!L78,"|",'Working Data'!M78)</f>
-        <v>stride_spearmint|Stride Spearmint|0|0|0|Mondelez International Kraft Foods Cadbury|Stride|Spearmint|?||United States|0|stride_spearmint.jpg</v>
+        <v>stride_spearmint|Stride Spearmint|0|1|0|Mondelez International Kraft Foods Cadbury|Stride|Spearmint|?||United States|0|stride_spearmint.jpg</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="str">
         <f>CONCATENATE('Working Data'!A79,"|",'Working Data'!B79,"|",'Working Data'!C79,"|",'Working Data'!D79,"|",'Working Data'!E79,"|",'Working Data'!F79,"|",'Working Data'!G79,"|",'Working Data'!H79,"|",'Working Data'!I79,"|",'Working Data'!J79,"|",'Working Data'!K79,"|",'Working Data'!L79,"|",'Working Data'!M79)</f>
-        <v>stride_sweet_peppermint|Stride Sweet Peppermint|0|0|0|Mondelez International Kraft Foods Cadbury|Stride|Sweet Peppermint|?||United States|0|stride_sweet_peppermint.jpg</v>
+        <v>stride_sweet_peppermint|Stride Sweet Peppermint|0|1|0|Mondelez International Kraft Foods Cadbury|Stride|Sweet Peppermint|?||United States|0|stride_sweet_peppermint.jpg</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="str">
         <f>CONCATENATE('Working Data'!A80,"|",'Working Data'!B80,"|",'Working Data'!C80,"|",'Working Data'!D80,"|",'Working Data'!E80,"|",'Working Data'!F80,"|",'Working Data'!G80,"|",'Working Data'!H80,"|",'Working Data'!I80,"|",'Working Data'!J80,"|",'Working Data'!K80,"|",'Working Data'!L80,"|",'Working Data'!M80)</f>
-        <v>stride_sweet_berry|Stride Sweet Berry|0|0|0|Mondelez International Kraft Foods Cadbury|Stride|Sweet Berry|?||United States|0|stride_sweet_berry.jpg</v>
+        <v>stride_sweet_berry|Stride Sweet Berry|0|1|0|Mondelez International Kraft Foods Cadbury|Stride|Sweet Berry|?||United States|0|stride_sweet_berry.jpg</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="str">
         <f>CONCATENATE('Working Data'!A81,"|",'Working Data'!B81,"|",'Working Data'!C81,"|",'Working Data'!D81,"|",'Working Data'!E81,"|",'Working Data'!F81,"|",'Working Data'!G81,"|",'Working Data'!H81,"|",'Working Data'!I81,"|",'Working Data'!J81,"|",'Working Data'!K81,"|",'Working Data'!L81,"|",'Working Data'!M81)</f>
-        <v>stride_uber_bubble|Stride Uber Bubble|0|0|0|Mondelez International Kraft Foods Cadbury|Stride|Uber Bubble|?||United States|0|stride_uber_bubble.jpg</v>
+        <v>stride_uber_bubble|Stride Uber Bubble|0|1|0|Mondelez International Kraft Foods Cadbury|Stride|Uber Bubble|?||United States|0|stride_uber_bubble.jpg</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="str">
         <f>CONCATENATE('Working Data'!A82,"|",'Working Data'!B82,"|",'Working Data'!C82,"|",'Working Data'!D82,"|",'Working Data'!E82,"|",'Working Data'!F82,"|",'Working Data'!G82,"|",'Working Data'!H82,"|",'Working Data'!I82,"|",'Working Data'!J82,"|",'Working Data'!K82,"|",'Working Data'!L82,"|",'Working Data'!M82)</f>
-        <v>stride_sweet_cinnamon|Stride Sweet Cinnamon|0|0|0|Mondelez International Kraft Foods Cadbury|Stride|Sweet Cinnamon|?||United States|0|stride_sweet_cinnamon.jpg</v>
+        <v>stride_sweet_cinnamon|Stride Sweet Cinnamon|0|1|0|Mondelez International Kraft Foods Cadbury|Stride|Sweet Cinnamon|?||United States|0|stride_sweet_cinnamon.jpg</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="str">
         <f>CONCATENATE('Working Data'!A83,"|",'Working Data'!B83,"|",'Working Data'!C83,"|",'Working Data'!D83,"|",'Working Data'!E83,"|",'Working Data'!F83,"|",'Working Data'!G83,"|",'Working Data'!H83,"|",'Working Data'!I83,"|",'Working Data'!J83,"|",'Working Data'!K83,"|",'Working Data'!L83,"|",'Working Data'!M83)</f>
-        <v>stride_forever_fruit|Stride Forever Fruit|0|0|0|Mondelez International Kraft Foods Cadbury|Stride|Forever Fruit|?||United States|0|stride_forever_fruit.jpg</v>
+        <v>stride_forever_fruit|Stride Forever Fruit|0|1|0|Mondelez International Kraft Foods Cadbury|Stride|Forever Fruit|?||United States|0|stride_forever_fruit.jpg</v>
       </c>
     </row>
     <row r="83" spans="1:1">
@@ -13823,7 +13846,7 @@
     <row r="97" spans="1:1">
       <c r="A97" t="str">
         <f>CONCATENATE('Working Data'!A98,"|",'Working Data'!B98,"|",'Working Data'!C98,"|",'Working Data'!D98,"|",'Working Data'!E98,"|",'Working Data'!F98,"|",'Working Data'!G98,"|",'Working Data'!H98,"|",'Working Data'!I98,"|",'Working Data'!J98,"|",'Working Data'!K98,"|",'Working Data'!L98,"|",'Working Data'!M98)</f>
-        <v>extra_fruit_sensations_strawberry_banana|Extra Fruit Sensations Strawberry Banana|022000108425|1|0|Mars Inc Wrigley|Extra Fruit Sensations|Strawberry Banana|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_fruit_sensations_strawberry_banana.png</v>
+        <v>extra_fruit_sensations_strawberry_banana|Extra Fruit Sensations Strawberry Banana|022000108425|1|0|Mars Inc Wrigley|Extra Fruit Sensations|Strawberry Banana|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_fruit_sensations_strawberry_banana.jpg</v>
       </c>
     </row>
     <row r="98" spans="1:1">
@@ -13919,7 +13942,7 @@
     <row r="113" spans="1:1">
       <c r="A113" t="str">
         <f>CONCATENATE('Working Data'!A114,"|",'Working Data'!B114,"|",'Working Data'!C114,"|",'Working Data'!D114,"|",'Working Data'!E114,"|",'Working Data'!F114,"|",'Working Data'!G114,"|",'Working Data'!H114,"|",'Working Data'!I114,"|",'Working Data'!J114,"|",'Working Data'!K114,"|",'Working Data'!L114,"|",'Working Data'!M114)</f>
-        <v>5_gum_swerve|5 Gum Swerve|022000013170|1|0|Mars Inc Wrigley|5 Gum|Swerve (TM)|a tangy to sweet tropical||United States|0|5_gum_swerve.jpg</v>
+        <v>5_gum_swerve|5 Gum Swerve|022000013170|1|0|Mars Inc Wrigley|5 Gum|Swerve (TM)|a tangy to sweet tropical||United States|0|5_gum_swerve.jpeg</v>
       </c>
     </row>
     <row r="114" spans="1:1">
@@ -13943,25 +13966,25 @@
     <row r="117" spans="1:1">
       <c r="A117" t="str">
         <f>CONCATENATE('Working Data'!A118,"|",'Working Data'!B118,"|",'Working Data'!C118,"|",'Working Data'!D118,"|",'Working Data'!E118,"|",'Working Data'!F118,"|",'Working Data'!G118,"|",'Working Data'!H118,"|",'Working Data'!I118,"|",'Working Data'!J118,"|",'Working Data'!K118,"|",'Working Data'!L118,"|",'Working Data'!M118)</f>
-        <v>5_gum_lush|5 Gum Lush|022000107237|1|1|Mars Inc Wrigley|5 Gum|Lush|a tangy to sweet tropical||United States|0|5_gum_lush.png</v>
+        <v>5_gum_lush|5 Gum Lush|022000107237|1|1|Mars Inc Wrigley|5 Gum|Lush|a tangy to sweet tropical||United States|0|5_gum_lush.jpg</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="str">
         <f>CONCATENATE('Working Data'!A119,"|",'Working Data'!B119,"|",'Working Data'!C119,"|",'Working Data'!D119,"|",'Working Data'!E119,"|",'Working Data'!F119,"|",'Working Data'!G119,"|",'Working Data'!H119,"|",'Working Data'!I119,"|",'Working Data'!J119,"|",'Working Data'!K119,"|",'Working Data'!L119,"|",'Working Data'!M119)</f>
-        <v>5_gum_zing|5 Gum Zing|022000112446|1|1|Mars Inc Wrigley|5 Gum|Zing|||United States|0|5_gum_zing.png</v>
+        <v>5_gum_zing|5 Gum Zing|022000112446|1|1|Mars Inc Wrigley|5 Gum|Zing|||United States|0|5_gum_zing.jpg</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="str">
         <f>CONCATENATE('Working Data'!A120,"|",'Working Data'!B120,"|",'Working Data'!C120,"|",'Working Data'!D120,"|",'Working Data'!E120,"|",'Working Data'!F120,"|",'Working Data'!G120,"|",'Working Data'!H120,"|",'Working Data'!I120,"|",'Working Data'!J120,"|",'Working Data'!K120,"|",'Working Data'!L120,"|",'Working Data'!M120)</f>
-        <v>wrigleys_winterfresh|Wrigley's Winterfresh|02266901|1|0|Mars Inc Wrigley|Wrigley's|Winterfresh|||United States|0|wrigleys_winterfresh</v>
+        <v>wrigleys_winterfresh|Wrigley's Winterfresh|02266901|1|0|Mars Inc Wrigley|Wrigley's|Winterfresh|||United States|0|wrigleys_winterfresh.png</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="str">
         <f>CONCATENATE('Working Data'!A121,"|",'Working Data'!B121,"|",'Working Data'!C121,"|",'Working Data'!D121,"|",'Working Data'!E121,"|",'Working Data'!F121,"|",'Working Data'!G121,"|",'Working Data'!H121,"|",'Working Data'!I121,"|",'Working Data'!J121,"|",'Working Data'!K121,"|",'Working Data'!L121,"|",'Working Data'!M121)</f>
-        <v>wrigleys_spearmint|Wrigley's Spearmint|02266500|1|0|Mars Inc Wrigley|Wrigley's|Spearmint|||United States|0|wrigleys_spearmint</v>
+        <v>wrigleys_spearmint|Wrigley's Spearmint|02266500|1|0|Mars Inc Wrigley|Wrigley's|Spearmint|||United States|0|wrigleys_spearmint.jpg</v>
       </c>
     </row>
     <row r="121" spans="1:1">
@@ -14040,6 +14063,468 @@
       <c r="A133" t="str">
         <f>CONCATENATE('Working Data'!A134,"|",'Working Data'!B134,"|",'Working Data'!C134,"|",'Working Data'!D134,"|",'Working Data'!E134,"|",'Working Data'!F134,"|",'Working Data'!G134,"|",'Working Data'!H134,"|",'Working Data'!I134,"|",'Working Data'!J134,"|",'Working Data'!K134,"|",'Working Data'!L134,"|",'Working Data'!M134)</f>
         <v>hubba_bubba_max_mystery_flavor|Hubba Bubba Max Mystery Flavor|0|1|0|Mars Inc Wrigley|Hubba Bubba Max|Mystery Flavor|||United States|0|hubba_bubba_max_mystery_flavor.jpg</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="str">
+        <f>CONCATENATE('Working Data'!A135,"|",'Working Data'!B135,"|",'Working Data'!C135,"|",'Working Data'!D135,"|",'Working Data'!E135,"|",'Working Data'!F135,"|",'Working Data'!G135,"|",'Working Data'!H135,"|",'Working Data'!I135,"|",'Working Data'!J135,"|",'Working Data'!K135,"|",'Working Data'!L135,"|",'Working Data'!M135)</f>
+        <v>hubba_bubba_squeeze_pop_assorted_sour_flavors|Hubba Bubba Squeeze Pop Assorted Sour Flavors|0|1|0|Mars Inc Wrigley|Hubba Bubba Squeeze Pop|Assorted Sour Flavors|||United States|0|hubba_bubba_squeeze_pop_assorted_sour_flavors.jpg</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="str">
+        <f>CONCATENATE('Working Data'!A136,"|",'Working Data'!B136,"|",'Working Data'!C136,"|",'Working Data'!D136,"|",'Working Data'!E136,"|",'Working Data'!F136,"|",'Working Data'!G136,"|",'Working Data'!H136,"|",'Working Data'!I136,"|",'Working Data'!J136,"|",'Working Data'!K136,"|",'Working Data'!L136,"|",'Working Data'!M136)</f>
+        <v>hubba_bubba_bubble_tape_awesome_original|Hubba Bubba Bubble Tape Awesome Original|022110079806|1|0|Mars Inc Wrigley|Hubba Bubba Bubble Tape|Awesome Original|||United States|0|hubba_bubba_bubble_tape_awesome_original.jpg</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="str">
+        <f>CONCATENATE('Working Data'!A137,"|",'Working Data'!B137,"|",'Working Data'!C137,"|",'Working Data'!D137,"|",'Working Data'!E137,"|",'Working Data'!F137,"|",'Working Data'!G137,"|",'Working Data'!H137,"|",'Working Data'!I137,"|",'Working Data'!J137,"|",'Working Data'!K137,"|",'Working Data'!L137,"|",'Working Data'!M137)</f>
+        <v>hubba_bubba_bubble_tape_snappy_strawberry|Hubba Bubba Bubble Tape Snappy Strawberry|0|1|0|Mars Inc Wrigley|Hubba Bubba Bubble Tape|Snappy Strawberry|||United States|0|hubba_bubba_bubble_tape_snappy_strawberry.jpg</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="str">
+        <f>CONCATENATE('Working Data'!A138,"|",'Working Data'!B138,"|",'Working Data'!C138,"|",'Working Data'!D138,"|",'Working Data'!E138,"|",'Working Data'!F138,"|",'Working Data'!G138,"|",'Working Data'!H138,"|",'Working Data'!I138,"|",'Working Data'!J138,"|",'Working Data'!K138,"|",'Working Data'!L138,"|",'Working Data'!M138)</f>
+        <v>hubba_bubba_bubble_tape_sour_apple|Hubba Bubba Bubble Tape Sour Apple|0|1|0|Mars Inc Wrigley|Hubba Bubba Bubble Tape|Sour Apple|||United States|0|hubba_bubba_bubble_tape_sour_apple.jpg</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="str">
+        <f>CONCATENATE('Working Data'!A139,"|",'Working Data'!B139,"|",'Working Data'!C139,"|",'Working Data'!D139,"|",'Working Data'!E139,"|",'Working Data'!F139,"|",'Working Data'!G139,"|",'Working Data'!H139,"|",'Working Data'!I139,"|",'Working Data'!J139,"|",'Working Data'!K139,"|",'Working Data'!L139,"|",'Working Data'!M139)</f>
+        <v>hubba_bubba_bubble_tape_triple_treat|Hubba Bubba Bubble Tape Triple Treat|0|1|0|Mars Inc Wrigley|Hubba Bubba Bubble Tape|Triple Treat|||United States|0|hubba_bubba_bubble_tape_triple_treat.jpg</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="str">
+        <f>CONCATENATE('Working Data'!A140,"|",'Working Data'!B140,"|",'Working Data'!C140,"|",'Working Data'!D140,"|",'Working Data'!E140,"|",'Working Data'!F140,"|",'Working Data'!G140,"|",'Working Data'!H140,"|",'Working Data'!I140,"|",'Working Data'!J140,"|",'Working Data'!K140,"|",'Working Data'!L140,"|",'Working Data'!M140)</f>
+        <v>hubba_bubba_bubble_tape_tangy_tropical|Hubba Bubba Bubble Tape Tangy Tropical|0|1|0|Mars Inc Wrigley|Hubba Bubba Bubble Tape|Tangy Tropical|||United States|0|hubba_bubba_bubble_tape_tangy_tropical.jpg</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="str">
+        <f>CONCATENATE('Working Data'!A141,"|",'Working Data'!B141,"|",'Working Data'!C141,"|",'Working Data'!D141,"|",'Working Data'!E141,"|",'Working Data'!F141,"|",'Working Data'!G141,"|",'Working Data'!H141,"|",'Working Data'!I141,"|",'Working Data'!J141,"|",'Working Data'!K141,"|",'Working Data'!L141,"|",'Working Data'!M141)</f>
+        <v>hubba_bubba_bubble_tape_mystery_flavor|Hubba Bubba Bubble Tape Mystery Flavor|0|1|0|Mars Inc Wrigley|Hubba Bubba Bubble Tape|Mystery Flavor|||United States|0|hubba_bubba_bubble_tape_mystery_flavor.jpeg</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" t="str">
+        <f>CONCATENATE('Working Data'!A142,"|",'Working Data'!B142,"|",'Working Data'!C142,"|",'Working Data'!D142,"|",'Working Data'!E142,"|",'Working Data'!F142,"|",'Working Data'!G142,"|",'Working Data'!H142,"|",'Working Data'!I142,"|",'Working Data'!J142,"|",'Working Data'!K142,"|",'Working Data'!L142,"|",'Working Data'!M142)</f>
+        <v>hubba_bubba_ouch_bubble_gum|Hubba Bubba OUCH! Bubble Gum|0|1|0|Mars Inc Wrigley|Hubba Bubba OUCH!|Bubble Gum|||United States|0|hubba_bubba_ouch_bubble_gum.jpg</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" t="str">
+        <f>CONCATENATE('Working Data'!A143,"|",'Working Data'!B143,"|",'Working Data'!C143,"|",'Working Data'!D143,"|",'Working Data'!E143,"|",'Working Data'!F143,"|",'Working Data'!G143,"|",'Working Data'!H143,"|",'Working Data'!I143,"|",'Working Data'!J143,"|",'Working Data'!K143,"|",'Working Data'!L143,"|",'Working Data'!M143)</f>
+        <v>wrigleys_juicy_fruit_juicy_secret|Wrigley's Juicy Fruit Juicy Secret|0|1|0|Mars Inc Wrigley|Wrigley's Juicy Fruit|Juicy Secret|||United States|0|wrigleys_juicy_fruit_juicy_secret.jpg</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" t="str">
+        <f>CONCATENATE('Working Data'!A144,"|",'Working Data'!B144,"|",'Working Data'!C144,"|",'Working Data'!D144,"|",'Working Data'!E144,"|",'Working Data'!F144,"|",'Working Data'!G144,"|",'Working Data'!H144,"|",'Working Data'!I144,"|",'Working Data'!J144,"|",'Working Data'!K144,"|",'Working Data'!L144,"|",'Working Data'!M144)</f>
+        <v>wrigleys_juicy_fruit_original|Wrigley's Juicy Fruit Original|02266707|1|0|Mars Inc Wrigley|Wrigley's Juicy Fruit|Original|||United States|0|wrigleys_juicy_fruit_original.jpg</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" t="str">
+        <f>CONCATENATE('Working Data'!A145,"|",'Working Data'!B145,"|",'Working Data'!C145,"|",'Working Data'!D145,"|",'Working Data'!E145,"|",'Working Data'!F145,"|",'Working Data'!G145,"|",'Working Data'!H145,"|",'Working Data'!I145,"|",'Working Data'!J145,"|",'Working Data'!K145,"|",'Working Data'!L145,"|",'Working Data'!M145)</f>
+        <v>wrigleys_juicy_fruit_sweet_fruit|Wrigley's Juicy Fruit Sweet Fruit|0|1|0|Mars Inc Wrigley|Wrigley's Juicy Fruit|Sweet Fruit|||United States|0|wrigleys_juicy_fruit_sweet_fruit.jpg</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="str">
+        <f>CONCATENATE('Working Data'!A146,"|",'Working Data'!B146,"|",'Working Data'!C146,"|",'Working Data'!D146,"|",'Working Data'!E146,"|",'Working Data'!F146,"|",'Working Data'!G146,"|",'Working Data'!H146,"|",'Working Data'!I146,"|",'Working Data'!J146,"|",'Working Data'!K146,"|",'Working Data'!L146,"|",'Working Data'!M146)</f>
+        <v>wrigleys_juicy_fruit_sweet_berry|Wrigley's Juicy Fruit Sweet Berry|0|1|0|Mars Inc Wrigley|Wrigley's Juicy Fruit|Sweet Berry|||United States|0|wrigleys_juicy_fruit_sweet_berry.jpg</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="str">
+        <f>CONCATENATE('Working Data'!A147,"|",'Working Data'!B147,"|",'Working Data'!C147,"|",'Working Data'!D147,"|",'Working Data'!E147,"|",'Working Data'!F147,"|",'Working Data'!G147,"|",'Working Data'!H147,"|",'Working Data'!I147,"|",'Working Data'!J147,"|",'Working Data'!K147,"|",'Working Data'!L147,"|",'Working Data'!M147)</f>
+        <v>wrigleys_juicy_fruit_groovy_fruity|Wrigley's Juicy Fruit Groovy Fruity|0|1|0|Mars Inc Wrigley|Wrigley's Juicy Fruit|Groovy Fruity|||United States|0|wrigleys_juicy_fruit_groovy_fruity.jpeg</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" t="str">
+        <f>CONCATENATE('Working Data'!A148,"|",'Working Data'!B148,"|",'Working Data'!C148,"|",'Working Data'!D148,"|",'Working Data'!E148,"|",'Working Data'!F148,"|",'Working Data'!G148,"|",'Working Data'!H148,"|",'Working Data'!I148,"|",'Working Data'!J148,"|",'Working Data'!K148,"|",'Working Data'!L148,"|",'Working Data'!M148)</f>
+        <v>orbit_peppermint|Orbit Peppermint|02248604|1|0|Mars Inc Wrigley|Orbit|Peppermint|||United States|0|orbit_peppermint.png</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="str">
+        <f>CONCATENATE('Working Data'!A149,"|",'Working Data'!B149,"|",'Working Data'!C149,"|",'Working Data'!D149,"|",'Working Data'!E149,"|",'Working Data'!F149,"|",'Working Data'!G149,"|",'Working Data'!H149,"|",'Working Data'!I149,"|",'Working Data'!J149,"|",'Working Data'!K149,"|",'Working Data'!L149,"|",'Working Data'!M149)</f>
+        <v>orbit_spearmint|Orbit Spearmint|022000013958 0224840|1|0|Mars Inc Wrigley|Orbit|Spearmint|||United States|0|orbit_spearmint.png</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="str">
+        <f>CONCATENATE('Working Data'!A150,"|",'Working Data'!B150,"|",'Working Data'!C150,"|",'Working Data'!D150,"|",'Working Data'!E150,"|",'Working Data'!F150,"|",'Working Data'!G150,"|",'Working Data'!H150,"|",'Working Data'!I150,"|",'Working Data'!J150,"|",'Working Data'!K150,"|",'Working Data'!L150,"|",'Working Data'!M150)</f>
+        <v>orbit_bubblemint|Orbit Bubblemint|02248905|1|0|Mars Inc Wrigley|Orbit|Bubblemint|||United States|0|orbit_bubblemint.png</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" t="str">
+        <f>CONCATENATE('Working Data'!A151,"|",'Working Data'!B151,"|",'Working Data'!C151,"|",'Working Data'!D151,"|",'Working Data'!E151,"|",'Working Data'!F151,"|",'Working Data'!G151,"|",'Working Data'!H151,"|",'Working Data'!I151,"|",'Working Data'!J151,"|",'Working Data'!K151,"|",'Working Data'!L151,"|",'Working Data'!M151)</f>
+        <v>orbit_wintermint|Orbit Wintermint|02248808|1|0|Mars Inc Wrigley|Orbit|Wintermint|||United States|0|orbit_wintermint.png</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" t="str">
+        <f>CONCATENATE('Working Data'!A152,"|",'Working Data'!B152,"|",'Working Data'!C152,"|",'Working Data'!D152,"|",'Working Data'!E152,"|",'Working Data'!F152,"|",'Working Data'!G152,"|",'Working Data'!H152,"|",'Working Data'!I152,"|",'Working Data'!J152,"|",'Working Data'!K152,"|",'Working Data'!L152,"|",'Working Data'!M152)</f>
+        <v>orbit_cinnamint|Orbit Cinnamint|02248507|1|0|Mars Inc Wrigley|Orbit|Cinnamint|||United States|0|orbit_cinnamint.png</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="str">
+        <f>CONCATENATE('Working Data'!A153,"|",'Working Data'!B153,"|",'Working Data'!C153,"|",'Working Data'!D153,"|",'Working Data'!E153,"|",'Working Data'!F153,"|",'Working Data'!G153,"|",'Working Data'!H153,"|",'Working Data'!I153,"|",'Working Data'!J153,"|",'Working Data'!K153,"|",'Working Data'!L153,"|",'Working Data'!M153)</f>
+        <v>orbit_sweetmint|Orbit Sweetmint|02248303|1|0|Mars Inc Wrigley|Orbit|Sweetmint|||United States|0|orbit_sweetmint.png</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" t="str">
+        <f>CONCATENATE('Working Data'!A154,"|",'Working Data'!B154,"|",'Working Data'!C154,"|",'Working Data'!D154,"|",'Working Data'!E154,"|",'Working Data'!F154,"|",'Working Data'!G154,"|",'Working Data'!H154,"|",'Working Data'!I154,"|",'Working Data'!J154,"|",'Working Data'!K154,"|",'Working Data'!L154,"|",'Working Data'!M154)</f>
+        <v>orbit_maui_melon_mint|Orbit Maui Melon Mint|0|1|0|Mars Inc Wrigley|Orbit|Maui Melon Mint|||United States|0|orbit_maui_melon_mint.png</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" t="str">
+        <f>CONCATENATE('Working Data'!A155,"|",'Working Data'!B155,"|",'Working Data'!C155,"|",'Working Data'!D155,"|",'Working Data'!E155,"|",'Working Data'!F155,"|",'Working Data'!G155,"|",'Working Data'!H155,"|",'Working Data'!I155,"|",'Working Data'!J155,"|",'Working Data'!K155,"|",'Working Data'!L155,"|",'Working Data'!M155)</f>
+        <v>orbit_wildberry_remix|Orbit Wildberry Remix|022000013347|1|0|Mars Inc Wrigley|Orbit|Wildberry Remix|||United States|0|orbit_wildberry_remix.png</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" t="str">
+        <f>CONCATENATE('Working Data'!A156,"|",'Working Data'!B156,"|",'Working Data'!C156,"|",'Working Data'!D156,"|",'Working Data'!E156,"|",'Working Data'!F156,"|",'Working Data'!G156,"|",'Working Data'!H156,"|",'Working Data'!I156,"|",'Working Data'!J156,"|",'Working Data'!K156,"|",'Working Data'!L156,"|",'Working Data'!M156)</f>
+        <v>orbit_melon_remix|Orbit Melon Remix|022000013743|1|0|Mars Inc Wrigley|Orbit|Melon Remix|||United States|0|orbit_melon_remix.png</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" t="str">
+        <f>CONCATENATE('Working Data'!A157,"|",'Working Data'!B157,"|",'Working Data'!C157,"|",'Working Data'!D157,"|",'Working Data'!E157,"|",'Working Data'!F157,"|",'Working Data'!G157,"|",'Working Data'!H157,"|",'Working Data'!I157,"|",'Working Data'!J157,"|",'Working Data'!K157,"|",'Working Data'!L157,"|",'Working Data'!M157)</f>
+        <v>orbit_tropical_remix|Orbit Tropical Remix|022000011794|1|0|Mars Inc Wrigley|Orbit|Tropical Remix|||United States|0|orbit_tropical_remix.png</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" t="str">
+        <f>CONCATENATE('Working Data'!A158,"|",'Working Data'!B158,"|",'Working Data'!C158,"|",'Working Data'!D158,"|",'Working Data'!E158,"|",'Working Data'!F158,"|",'Working Data'!G158,"|",'Working Data'!H158,"|",'Working Data'!I158,"|",'Working Data'!J158,"|",'Working Data'!K158,"|",'Working Data'!L158,"|",'Working Data'!M158)</f>
+        <v>orbit_strawberry_remix|Orbit Strawberry Remix|0|1|0|Mars Inc Wrigley|Orbit|Strawberry Remix|||United States|0|orbit_strawberry_remix.png</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" t="str">
+        <f>CONCATENATE('Working Data'!A159,"|",'Working Data'!B159,"|",'Working Data'!C159,"|",'Working Data'!D159,"|",'Working Data'!E159,"|",'Working Data'!F159,"|",'Working Data'!G159,"|",'Working Data'!H159,"|",'Working Data'!I159,"|",'Working Data'!J159,"|",'Working Data'!K159,"|",'Working Data'!L159,"|",'Working Data'!M159)</f>
+        <v>orbit_mist_raspberry_lemon_dew|Orbit Mist Raspberry Lemon Dew|022000113795|1|0|Mars Inc Wrigley|Orbit Mist|Raspberry Lemon Dew|The smooth, refreshing flavor of sugar-free Orbit gum leaves your mouth with a "just brushed clean feeling".||United States|0|orbit_mist_raspberry_lemon_dew.jpg</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" t="str">
+        <f>CONCATENATE('Working Data'!A160,"|",'Working Data'!B160,"|",'Working Data'!C160,"|",'Working Data'!D160,"|",'Working Data'!E160,"|",'Working Data'!F160,"|",'Working Data'!G160,"|",'Working Data'!H160,"|",'Working Data'!I160,"|",'Working Data'!J160,"|",'Working Data'!K160,"|",'Working Data'!L160,"|",'Working Data'!M160)</f>
+        <v>orbit_mist_peppermint_spray|Orbit Mist Peppermint Spray|022000110435|1|0|Mars Inc Wrigley|Orbit Mist|Peppermint Spray|The smooth, refreshing flavor of sugar-free Orbit gum leaves your mouth with a "just brushed clean feeling".||United States|0|orbit_mist_peppermint_spray.jpg</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" t="str">
+        <f>CONCATENATE('Working Data'!A161,"|",'Working Data'!B161,"|",'Working Data'!C161,"|",'Working Data'!D161,"|",'Working Data'!E161,"|",'Working Data'!F161,"|",'Working Data'!G161,"|",'Working Data'!H161,"|",'Working Data'!I161,"|",'Working Data'!J161,"|",'Working Data'!K161,"|",'Working Data'!L161,"|",'Working Data'!M161)</f>
+        <v>orbit_mist_spearmint_spritzer|Orbit Mist Spearmint Spritzer|022000115577|1|0|Mars Inc Wrigley|Orbit Mist|Spearmint Spritzer|The smooth, refreshing flavor of sugar-free Orbit gum leaves your mouth with a "just brushed clean feeling".||United States|0|orbit_mist_spearmint_spritzer.jpg</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" t="str">
+        <f>CONCATENATE('Working Data'!A162,"|",'Working Data'!B162,"|",'Working Data'!C162,"|",'Working Data'!D162,"|",'Working Data'!E162,"|",'Working Data'!F162,"|",'Working Data'!G162,"|",'Working Data'!H162,"|",'Working Data'!I162,"|",'Working Data'!J162,"|",'Working Data'!K162,"|",'Working Data'!L162,"|",'Working Data'!M162)</f>
+        <v>orbit_mist_watermelon_spring|Orbit Mist Watermelon Spring|022000110398|1|0|Mars Inc Wrigley|Orbit Mist|Watermelon Spring|The smooth, refreshing flavor of sugar-free Orbit gum leaves your mouth with a "just brushed clean feeling".||United States|0|orbit_mist_watermelon_spring.jpg</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" t="str">
+        <f>CONCATENATE('Working Data'!A163,"|",'Working Data'!B163,"|",'Working Data'!C163,"|",'Working Data'!D163,"|",'Working Data'!E163,"|",'Working Data'!F163,"|",'Working Data'!G163,"|",'Working Data'!H163,"|",'Working Data'!I163,"|",'Working Data'!J163,"|",'Working Data'!K163,"|",'Working Data'!L163,"|",'Working Data'!M163)</f>
+        <v>orbit_mist_crisp_mint_waterfall|Orbit Mist Crisp Mint Waterfall|022000119704|1|0|Mars Inc Wrigley|Orbit Mist|Crisp Mint Waterfall|The smooth, refreshing flavor of sugar-free Orbit gum leaves your mouth with a "just brushed clean feeling".||United States|0|orbit_mist_crisp_mint_waterfall.jpg</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" t="str">
+        <f>CONCATENATE('Working Data'!A164,"|",'Working Data'!B164,"|",'Working Data'!C164,"|",'Working Data'!D164,"|",'Working Data'!E164,"|",'Working Data'!F164,"|",'Working Data'!G164,"|",'Working Data'!H164,"|",'Working Data'!I164,"|",'Working Data'!J164,"|",'Working Data'!K164,"|",'Working Data'!L164,"|",'Working Data'!M164)</f>
+        <v>orbit_white_bubblemint|Orbit White Bubblemint|0|1|0|Mars Inc Wrigley|Orbit White|Bubblemint|||United States|0|orbit_white_bubblemint.png</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" t="str">
+        <f>CONCATENATE('Working Data'!A165,"|",'Working Data'!B165,"|",'Working Data'!C165,"|",'Working Data'!D165,"|",'Working Data'!E165,"|",'Working Data'!F165,"|",'Working Data'!G165,"|",'Working Data'!H165,"|",'Working Data'!I165,"|",'Working Data'!J165,"|",'Working Data'!K165,"|",'Working Data'!L165,"|",'Working Data'!M165)</f>
+        <v>orbit_white_peppermint|Orbit White Peppermint|0|1|0|Mars Inc Wrigley|Orbit White|Peppermint|||United States|0|orbit_white_peppermint.png</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" t="str">
+        <f>CONCATENATE('Working Data'!A166,"|",'Working Data'!B166,"|",'Working Data'!C166,"|",'Working Data'!D166,"|",'Working Data'!E166,"|",'Working Data'!F166,"|",'Working Data'!G166,"|",'Working Data'!H166,"|",'Working Data'!I166,"|",'Working Data'!J166,"|",'Working Data'!K166,"|",'Working Data'!L166,"|",'Working Data'!M166)</f>
+        <v>orbit_white_spearmint|Orbit White Spearmint|0|1|0|Mars Inc Wrigley|Orbit White|Spearmint|||United States|0|orbit_white_spearmint.png</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" t="str">
+        <f>CONCATENATE('Working Data'!A167,"|",'Working Data'!B167,"|",'Working Data'!C167,"|",'Working Data'!D167,"|",'Working Data'!E167,"|",'Working Data'!F167,"|",'Working Data'!G167,"|",'Working Data'!H167,"|",'Working Data'!I167,"|",'Working Data'!J167,"|",'Working Data'!K167,"|",'Working Data'!L167,"|",'Working Data'!M167)</f>
+        <v>id_peppermint|iD Peppermint|012546685115|1|0|Mondelez International Kraft Foods Cadbury|iD|Peppermint|iD Gum puts a delicious twist on the flavors you love, like Peppermint, BerryMelon and Spearmint. Each pack features unique artwork created by emerging artists, making it kinda a pack of gum and kinda a breathtakingly moving masterpiece. Not to mention a magnetic closure that helps keep your gum secure in the pack. And that's just the beginning.|Kinda tastes like peppermint and kinda like a hint of something else. iD Gum. Kinda more than gum. Kinda amazing.|United States|0|id_peppermint.png</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" t="str">
+        <f>CONCATENATE('Working Data'!A168,"|",'Working Data'!B168,"|",'Working Data'!C168,"|",'Working Data'!D168,"|",'Working Data'!E168,"|",'Working Data'!F168,"|",'Working Data'!G168,"|",'Working Data'!H168,"|",'Working Data'!I168,"|",'Working Data'!J168,"|",'Working Data'!K168,"|",'Working Data'!L168,"|",'Working Data'!M168)</f>
+        <v>id_spearmint|iD Spearmint|012546685061|1|0|Mondelez International Kraft Foods Cadbury|iD|Spearmint|iD Gum puts a delicious twist on the flavors you love, like Peppermint, BerryMelon and Spearmint. Each pack features unique artwork created by emerging artists, making it kinda a pack of gum and kinda a breathtakingly moving masterpiece. Not to mention a magnetic closure that helps keep your gum secure in the pack. And that's just the beginning.|Kinda tastes like spearmint and kinda has a little more to it. iD Gum. Kinda more than gum. Kinda amazing.|United States|0|id_spearmint.png</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" t="str">
+        <f>CONCATENATE('Working Data'!A169,"|",'Working Data'!B169,"|",'Working Data'!C169,"|",'Working Data'!D169,"|",'Working Data'!E169,"|",'Working Data'!F169,"|",'Working Data'!G169,"|",'Working Data'!H169,"|",'Working Data'!I169,"|",'Working Data'!J169,"|",'Working Data'!K169,"|",'Working Data'!L169,"|",'Working Data'!M169)</f>
+        <v>id_berrymelon|iD BerryMelon|012546685016|1|0|Mondelez International Kraft Foods Cadbury|iD|BerryMelon|iD Gum puts a delicious twist on the flavors you love, like Peppermint, BerryMelon and Spearmint. Each pack features unique artwork created by emerging artists, making it kinda a pack of gum and kinda a breathtakingly moving masterpiece. Not to mention a magnetic closure that helps keep your gum secure in the pack. And that's just the beginning.|Kinda tastes like berry and kinda tastes like watermelon. iD Gum. Kinda more than gum. Kinda amazing.|United States|0|id_berrymelon.png</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" t="str">
+        <f>CONCATENATE('Working Data'!A170,"|",'Working Data'!B170,"|",'Working Data'!C170,"|",'Working Data'!D170,"|",'Working Data'!E170,"|",'Working Data'!F170,"|",'Working Data'!G170,"|",'Working Data'!H170,"|",'Working Data'!I170,"|",'Working Data'!J170,"|",'Working Data'!K170,"|",'Working Data'!L170,"|",'Working Data'!M170)</f>
+        <v>up2u_daylight_mint_mintnight_mint|UP2U Daylight Mint / Mintnight Mint||1|0|Perfetti Van Melle Mentos|UP2U|Daylight Mint / Mintnight Mint|Two juicy mint flavors in one pack. One for day. One for night.||United States|0|up2u_daylight_mint_mintnight_mint.png</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" t="str">
+        <f>CONCATENATE('Working Data'!A171,"|",'Working Data'!B171,"|",'Working Data'!C171,"|",'Working Data'!D171,"|",'Working Data'!E171,"|",'Working Data'!F171,"|",'Working Data'!G171,"|",'Working Data'!H171,"|",'Working Data'!I171,"|",'Working Data'!J171,"|",'Working Data'!K171,"|",'Working Data'!L171,"|",'Working Data'!M171)</f>
+        <v>up2u_berry_watermelon_fresh_mint|UP2U Berry Watermelon / Fresh Mint|073390014001|1|0|Perfetti Van Melle Mentos|UP2U|Berry Watermelon / Fresh Mint|We mashed two frutis together and paired them with a crisp mint. They like each other.||United States|0|up2u_berry_watermelon_fresh_mint.png</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" t="str">
+        <f>CONCATENATE('Working Data'!A172,"|",'Working Data'!B172,"|",'Working Data'!C172,"|",'Working Data'!D172,"|",'Working Data'!E172,"|",'Working Data'!F172,"|",'Working Data'!G172,"|",'Working Data'!H172,"|",'Working Data'!I172,"|",'Working Data'!J172,"|",'Working Data'!K172,"|",'Working Data'!L172,"|",'Working Data'!M172)</f>
+        <v>up2u_striped_red_strawberry_starmint|UP2U Striped Red Strawberry / Starmint|073390013998|1|0|Perfetti Van Melle Mentos|UP2U|Striped Red Strawberry / Starmint|Big, gorgeous strawberry deliciousness as American as apple pie, except for the apple part. Paired with the crisp minty'ness of outer space.||United States|0|up2u_striped_red_strawberry_starmint.png</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" t="str">
+        <f>CONCATENATE('Working Data'!A173,"|",'Working Data'!B173,"|",'Working Data'!C173,"|",'Working Data'!D173,"|",'Working Data'!E173,"|",'Working Data'!F173,"|",'Working Data'!G173,"|",'Working Data'!H173,"|",'Working Data'!I173,"|",'Working Data'!J173,"|",'Working Data'!K173,"|",'Working Data'!L173,"|",'Working Data'!M173)</f>
+        <v>up2u_superfruit_smasher_tropical_mixer|UP2U Superfruit Smasher / Tropical Mixer||1|0|Perfetti Van Melle Mentos|UP2U|Superfruit Smasher / Tropical Mixer|Superfruit is a mashed-up blend of mouth-watering goodness.  On the other side, more fruit goodness, this time of the tropical variety.||United States|0|up2u_superfruit_smasher_tropical_mixer.png</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" t="str">
+        <f>CONCATENATE('Working Data'!A174,"|",'Working Data'!B174,"|",'Working Data'!C174,"|",'Working Data'!D174,"|",'Working Data'!E174,"|",'Working Data'!F174,"|",'Working Data'!G174,"|",'Working Data'!H174,"|",'Working Data'!I174,"|",'Working Data'!J174,"|",'Working Data'!K174,"|",'Working Data'!L174,"|",'Working Data'!M174)</f>
+        <v>up2u_energy_strike_chillax_mint|UP2U Energy Strike / Chillax Mint||1|0|Perfetti Van Melle Mentos|UP2U|Energy Strike / Chillax Mint|With a boost of flavor on one side and a relaxing blend on the other, you're all set for whatever mood you're feeling.||United States|0|up2u_energy_strike_chillax_mint.png</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" t="str">
+        <f>CONCATENATE('Working Data'!A175,"|",'Working Data'!B175,"|",'Working Data'!C175,"|",'Working Data'!D175,"|",'Working Data'!E175,"|",'Working Data'!F175,"|",'Working Data'!G175,"|",'Working Data'!H175,"|",'Working Data'!I175,"|",'Working Data'!J175,"|",'Working Data'!K175,"|",'Working Data'!L175,"|",'Working Data'!M175)</f>
+        <v>up2u_mandarin_strawberry_spearmint|UP2U Mandarin Strawberry / Spearmint||1|0|Perfetti Van Melle Mentos|UP2U|Mandarin Strawberry / Spearmint|Delicious citrus and strawberry living alongside a classic spearmint in harmony.||United States|0|up2u_mandarin_strawberry_spearmint.png</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" t="str">
+        <f>CONCATENATE('Working Data'!A176,"|",'Working Data'!B176,"|",'Working Data'!C176,"|",'Working Data'!D176,"|",'Working Data'!E176,"|",'Working Data'!F176,"|",'Working Data'!G176,"|",'Working Data'!H176,"|",'Working Data'!I176,"|",'Working Data'!J176,"|",'Working Data'!K176,"|",'Working Data'!L176,"|",'Working Data'!M176)</f>
+        <v>up2u_sweet_mint_bubble_fresh|UP2U Sweet Mint / Bubble Fresh|073390014018|1|0|Perfetti Van Melle Mentos|UP2U|Sweet Mint / Bubble Fresh|Mint with a hint of sweet, snuggled up to yummy bubble gum.  And snuggle they do.||United States|0|up2u_sweet_mint_bubble_fresh.png</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" t="str">
+        <f>CONCATENATE('Working Data'!A177,"|",'Working Data'!B177,"|",'Working Data'!C177,"|",'Working Data'!D177,"|",'Working Data'!E177,"|",'Working Data'!F177,"|",'Working Data'!G177,"|",'Working Data'!H177,"|",'Working Data'!I177,"|",'Working Data'!J177,"|",'Working Data'!K177,"|",'Working Data'!L177,"|",'Working Data'!M177)</f>
+        <v>bubblicious_watermelon|Bubblicious Watermelon|012546917582|1|0||Bubblicious|Watermelon|||United States|0|</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" t="str">
+        <f>CONCATENATE('Working Data'!A178,"|",'Working Data'!B178,"|",'Working Data'!C178,"|",'Working Data'!D178,"|",'Working Data'!E178,"|",'Working Data'!F178,"|",'Working Data'!G178,"|",'Working Data'!H178,"|",'Working Data'!I178,"|",'Working Data'!J178,"|",'Working Data'!K178,"|",'Working Data'!L178,"|",'Working Data'!M178)</f>
+        <v>hubba_bubba_crush_orange|Hubba Bubba Crush Orange|022000015587|1|0||Hubba Bubba|Crush Orange|||United States|0|</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" t="str">
+        <f>CONCATENATE('Working Data'!A179,"|",'Working Data'!B179,"|",'Working Data'!C179,"|",'Working Data'!D179,"|",'Working Data'!E179,"|",'Working Data'!F179,"|",'Working Data'!G179,"|",'Working Data'!H179,"|",'Working Data'!I179,"|",'Working Data'!J179,"|",'Working Data'!K179,"|",'Working Data'!L179,"|",'Working Data'!M179)</f>
+        <v>hubba_bubba_dr_pepper|Hubba Bubba Dr. Pepper|022000015594|1|0||Hubba Bubba|Dr. Pepper|||United States|0|</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" t="str">
+        <f>CONCATENATE('Working Data'!A180,"|",'Working Data'!B180,"|",'Working Data'!C180,"|",'Working Data'!D180,"|",'Working Data'!E180,"|",'Working Data'!F180,"|",'Working Data'!G180,"|",'Working Data'!H180,"|",'Working Data'!I180,"|",'Working Data'!J180,"|",'Working Data'!K180,"|",'Working Data'!L180,"|",'Working Data'!M180)</f>
+        <v>ice_breakers_ice_cubes_peppermint|ICE BREAKERS (R) Ice Cubes (R) Peppermint|03484308 034000700028|1|0||ICE BREAKERS (R) Ice Cubes (R)|Peppermint|Treat your mouth to refreshingly delicious ICE BREAKERS ICE CUBES gum! These frosty cube-shaped pieces of gum are instantly cold and loaded with dazzling flavor crystals. ICE CUBES gum is available in intense mint and sweet fruit flavors.||United States|0|</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" t="str">
+        <f>CONCATENATE('Working Data'!A181,"|",'Working Data'!B181,"|",'Working Data'!C181,"|",'Working Data'!D181,"|",'Working Data'!E181,"|",'Working Data'!F181,"|",'Working Data'!G181,"|",'Working Data'!H181,"|",'Working Data'!I181,"|",'Working Data'!J181,"|",'Working Data'!K181,"|",'Working Data'!L181,"|",'Working Data'!M181)</f>
+        <v>ice_breakers_ice_cubes_spearmint|ICE BREAKERS (R) Ice Cubes (R) Spearmint|034000700035|1|0||ICE BREAKERS (R) Ice Cubes (R)|Spearmint|Treat your mouth to refreshingly delicious ICE BREAKERS ICE CUBES gum! These frosty cube-shaped pieces of gum are instantly cold and loaded with dazzling flavor crystals. ICE CUBES gum is available in intense mint and sweet fruit flavors.||United States|0|</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" t="str">
+        <f>CONCATENATE('Working Data'!A182,"|",'Working Data'!B182,"|",'Working Data'!C182,"|",'Working Data'!D182,"|",'Working Data'!E182,"|",'Working Data'!F182,"|",'Working Data'!G182,"|",'Working Data'!H182,"|",'Working Data'!I182,"|",'Working Data'!J182,"|",'Working Data'!K182,"|",'Working Data'!L182,"|",'Working Data'!M182)</f>
+        <v>ice_breakers_ice_cubes_rasberry_sorbet|ICE BREAKERS (R) Ice Cubes (R) Rasberry Sorbet|034000700271|1|0||ICE BREAKERS (R) Ice Cubes (R)|Rasberry Sorbet|Treat your mouth to refreshingly delicious ICE BREAKERS ICE CUBES gum! These frosty cube-shaped pieces of gum are instantly cold and loaded with dazzling flavor crystals. ICE CUBES gum is available in intense mint and sweet fruit flavors.||United States|0|</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" t="str">
+        <f>CONCATENATE('Working Data'!A183,"|",'Working Data'!B183,"|",'Working Data'!C183,"|",'Working Data'!D183,"|",'Working Data'!E183,"|",'Working Data'!F183,"|",'Working Data'!G183,"|",'Working Data'!H183,"|",'Working Data'!I183,"|",'Working Data'!J183,"|",'Working Data'!K183,"|",'Working Data'!L183,"|",'Working Data'!M183)</f>
+        <v>ice_breakers_ice_cubes_kiwi_watermelon |ICE BREAKERS (R) Ice Cubes (R) Kiwi Watermelon |034000700189|1|0||ICE BREAKERS (R) Ice Cubes (R)|Kiwi Watermelon |Treat your mouth to refreshingly delicious ICE BREAKERS ICE CUBES gum! These frosty cube-shaped pieces of gum are instantly cold and loaded with dazzling flavor crystals. ICE CUBES gum is available in intense mint and sweet fruit flavors.||United States|0|</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" t="str">
+        <f>CONCATENATE('Working Data'!A184,"|",'Working Data'!B184,"|",'Working Data'!C184,"|",'Working Data'!D184,"|",'Working Data'!E184,"|",'Working Data'!F184,"|",'Working Data'!G184,"|",'Working Data'!H184,"|",'Working Data'!I184,"|",'Working Data'!J184,"|",'Working Data'!K184,"|",'Working Data'!L184,"|",'Working Data'!M184)</f>
+        <v>ice_breakers_ice_cubes_strawberry_smoothie_gum|ICE BREAKERS (R) Ice Cubes (R) Strawberry Smoothie Gum|034000700172|1|0||ICE BREAKERS (R) Ice Cubes (R)|Strawberry Smoothie Gum|Treat your mouth to refreshingly delicious ICE BREAKERS ICE CUBES gum! These frosty cube-shaped pieces of gum are instantly cold and loaded with dazzling flavor crystals. ICE CUBES gum is available in intense mint and sweet fruit flavors.||United States|0|</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" t="str">
+        <f>CONCATENATE('Working Data'!A185,"|",'Working Data'!B185,"|",'Working Data'!C185,"|",'Working Data'!D185,"|",'Working Data'!E185,"|",'Working Data'!F185,"|",'Working Data'!G185,"|",'Working Data'!H185,"|",'Working Data'!I185,"|",'Working Data'!J185,"|",'Working Data'!K185,"|",'Working Data'!L185,"|",'Working Data'!M185)</f>
+        <v>ice_breakers_ice_cubes_wintergreen|ICE BREAKERS (R) Ice Cubes (R) Wintergreen|03452901|1|0||ICE BREAKERS (R) Ice Cubes (R)|Wintergreen|Treat your mouth to refreshingly delicious ICE BREAKERS ICE CUBES gum! These frosty cube-shaped pieces of gum are instantly cold and loaded with dazzling flavor crystals. ICE CUBES gum is available in intense mint and sweet fruit flavors.||United States|0|</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" t="str">
+        <f>CONCATENATE('Working Data'!A186,"|",'Working Data'!B186,"|",'Working Data'!C186,"|",'Working Data'!D186,"|",'Working Data'!E186,"|",'Working Data'!F186,"|",'Working Data'!G186,"|",'Working Data'!H186,"|",'Working Data'!I186,"|",'Working Data'!J186,"|",'Working Data'!K186,"|",'Working Data'!L186,"|",'Working Data'!M186)</f>
+        <v>ice_breakers_ice_cubes_cool_lemon|ICE BREAKERS (R) Ice Cubes (R) Cool Lemon (R)|03462005|1|0||ICE BREAKERS (R) Ice Cubes (R)|Cool Lemon (R)|Treat your mouth to refreshingly delicious ICE BREAKERS ICE CUBES gum! These frosty cube-shaped pieces of gum are instantly cold and loaded with dazzling flavor crystals. ICE CUBES gum is available in intense mint and sweet fruit flavors.||United States|0|</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" t="str">
+        <f>CONCATENATE('Working Data'!A187,"|",'Working Data'!B187,"|",'Working Data'!C187,"|",'Working Data'!D187,"|",'Working Data'!E187,"|",'Working Data'!F187,"|",'Working Data'!G187,"|",'Working Data'!H187,"|",'Working Data'!I187,"|",'Working Data'!J187,"|",'Working Data'!K187,"|",'Working Data'!L187,"|",'Working Data'!M187)</f>
+        <v>ice_breakers_ice_cubes_bubble_breeze|ICE BREAKERS (R) Ice Cubes (R) Bubble Breeze (R)|03464508|1|0||ICE BREAKERS (R) Ice Cubes (R)|Bubble Breeze (R)|Treat your mouth to refreshingly delicious ICE BREAKERS ICE CUBES gum! These frosty cube-shaped pieces of gum are instantly cold and loaded with dazzling flavor crystals. ICE CUBES gum is available in intense mint and sweet fruit flavors.||United States|0|</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" t="str">
+        <f>CONCATENATE('Working Data'!A188,"|",'Working Data'!B188,"|",'Working Data'!C188,"|",'Working Data'!D188,"|",'Working Data'!E188,"|",'Working Data'!F188,"|",'Working Data'!G188,"|",'Working Data'!H188,"|",'Working Data'!I188,"|",'Working Data'!J188,"|",'Working Data'!K188,"|",'Working Data'!L188,"|",'Working Data'!M188)</f>
+        <v>ice_breakers_ice_cubes_white_mango_kiwi_cooler|ICE BREAKERS (R) Ice Cubes (R) White Mango Kiwi Cooler|034000700363|1|0||ICE BREAKERS (R) Ice Cubes (R) White|Mango Kiwi Cooler|||||</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" t="str">
+        <f>CONCATENATE('Working Data'!A189,"|",'Working Data'!B189,"|",'Working Data'!C189,"|",'Working Data'!D189,"|",'Working Data'!E189,"|",'Working Data'!F189,"|",'Working Data'!G189,"|",'Working Data'!H189,"|",'Working Data'!I189,"|",'Working Data'!J189,"|",'Working Data'!K189,"|",'Working Data'!L189,"|",'Working Data'!M189)</f>
+        <v>ice_breakers_ice_cubes_white_winter_green_splash|ICE BREAKERS (R) Ice Cubes (R) White Winter Green Splash|034000700417|1|0||ICE BREAKERS (R) Ice Cubes (R) White|Winter Green Splash|||||</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" t="str">
+        <f>CONCATENATE('Working Data'!A190,"|",'Working Data'!B190,"|",'Working Data'!C190,"|",'Working Data'!D190,"|",'Working Data'!E190,"|",'Working Data'!F190,"|",'Working Data'!G190,"|",'Working Data'!H190,"|",'Working Data'!I190,"|",'Working Data'!J190,"|",'Working Data'!K190,"|",'Working Data'!L190,"|",'Working Data'!M190)</f>
+        <v>ice_breakers_stick_gum_coolmint|ICE BREAKERS (R) Stick Gum Coolmint|034000717804|1|0||ICE BREAKERS (R) Stick Gum|Coolmint|||||</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" t="str">
+        <f>CONCATENATE('Working Data'!A191,"|",'Working Data'!B191,"|",'Working Data'!C191,"|",'Working Data'!D191,"|",'Working Data'!E191,"|",'Working Data'!F191,"|",'Working Data'!G191,"|",'Working Data'!H191,"|",'Working Data'!I191,"|",'Working Data'!J191,"|",'Working Data'!K191,"|",'Working Data'!L191,"|",'Working Data'!M191)</f>
+        <v>ice_breakers_stick_gum_wintergreen|ICE BREAKERS (R) Stick Gum Wintergreen|034000717811|1|0||ICE BREAKERS (R) Stick Gum|Wintergreen|||||</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" t="str">
+        <f>CONCATENATE('Working Data'!A192,"|",'Working Data'!B192,"|",'Working Data'!C192,"|",'Working Data'!D192,"|",'Working Data'!E192,"|",'Working Data'!F192,"|",'Working Data'!G192,"|",'Working Data'!H192,"|",'Working Data'!I192,"|",'Working Data'!J192,"|",'Working Data'!K192,"|",'Working Data'!L192,"|",'Working Data'!M192)</f>
+        <v>_| |||0||||||||</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" t="str">
+        <f>CONCATENATE('Working Data'!A193,"|",'Working Data'!B193,"|",'Working Data'!C193,"|",'Working Data'!D193,"|",'Working Data'!E193,"|",'Working Data'!F193,"|",'Working Data'!G193,"|",'Working Data'!H193,"|",'Working Data'!I193,"|",'Working Data'!J193,"|",'Working Data'!K193,"|",'Working Data'!L193,"|",'Working Data'!M193)</f>
+        <v>_| |||||||||||</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" t="str">
+        <f>CONCATENATE('Working Data'!A194,"|",'Working Data'!B194,"|",'Working Data'!C194,"|",'Working Data'!D194,"|",'Working Data'!E194,"|",'Working Data'!F194,"|",'Working Data'!G194,"|",'Working Data'!H194,"|",'Working Data'!I194,"|",'Working Data'!J194,"|",'Working Data'!K194,"|",'Working Data'!L194,"|",'Working Data'!M194)</f>
+        <v>_| |||||||||||</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" t="str">
+        <f>CONCATENATE('Working Data'!A195,"|",'Working Data'!B195,"|",'Working Data'!C195,"|",'Working Data'!D195,"|",'Working Data'!E195,"|",'Working Data'!F195,"|",'Working Data'!G195,"|",'Working Data'!H195,"|",'Working Data'!I195,"|",'Working Data'!J195,"|",'Working Data'!K195,"|",'Working Data'!L195,"|",'Working Data'!M195)</f>
+        <v>_| |||||||||||</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" t="str">
+        <f>CONCATENATE('Working Data'!A196,"|",'Working Data'!B196,"|",'Working Data'!C196,"|",'Working Data'!D196,"|",'Working Data'!E196,"|",'Working Data'!F196,"|",'Working Data'!G196,"|",'Working Data'!H196,"|",'Working Data'!I196,"|",'Working Data'!J196,"|",'Working Data'!K196,"|",'Working Data'!L196,"|",'Working Data'!M196)</f>
+        <v>_| |||||||||||</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" t="str">
+        <f>CONCATENATE('Working Data'!A197,"|",'Working Data'!B197,"|",'Working Data'!C197,"|",'Working Data'!D197,"|",'Working Data'!E197,"|",'Working Data'!F197,"|",'Working Data'!G197,"|",'Working Data'!H197,"|",'Working Data'!I197,"|",'Working Data'!J197,"|",'Working Data'!K197,"|",'Working Data'!L197,"|",'Working Data'!M197)</f>
+        <v>_| |||||||||||</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" t="str">
+        <f>CONCATENATE('Working Data'!A198,"|",'Working Data'!B198,"|",'Working Data'!C198,"|",'Working Data'!D198,"|",'Working Data'!E198,"|",'Working Data'!F198,"|",'Working Data'!G198,"|",'Working Data'!H198,"|",'Working Data'!I198,"|",'Working Data'!J198,"|",'Working Data'!K198,"|",'Working Data'!L198,"|",'Working Data'!M198)</f>
+        <v>_| |||||||||||</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" t="str">
+        <f>CONCATENATE('Working Data'!A199,"|",'Working Data'!B199,"|",'Working Data'!C199,"|",'Working Data'!D199,"|",'Working Data'!E199,"|",'Working Data'!F199,"|",'Working Data'!G199,"|",'Working Data'!H199,"|",'Working Data'!I199,"|",'Working Data'!J199,"|",'Working Data'!K199,"|",'Working Data'!L199,"|",'Working Data'!M199)</f>
+        <v>_| |||||||||||</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" t="str">
+        <f>CONCATENATE('Working Data'!A200,"|",'Working Data'!B200,"|",'Working Data'!C200,"|",'Working Data'!D200,"|",'Working Data'!E200,"|",'Working Data'!F200,"|",'Working Data'!G200,"|",'Working Data'!H200,"|",'Working Data'!I200,"|",'Working Data'!J200,"|",'Working Data'!K200,"|",'Working Data'!L200,"|",'Working Data'!M200)</f>
+        <v>_| |||||||||||</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" t="str">
+        <f>CONCATENATE('Working Data'!A201,"|",'Working Data'!B201,"|",'Working Data'!C201,"|",'Working Data'!D201,"|",'Working Data'!E201,"|",'Working Data'!F201,"|",'Working Data'!G201,"|",'Working Data'!H201,"|",'Working Data'!I201,"|",'Working Data'!J201,"|",'Working Data'!K201,"|",'Working Data'!L201,"|",'Working Data'!M201)</f>
+        <v>_| |||||||||||</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" t="str">
+        <f>CONCATENATE('Working Data'!A202,"|",'Working Data'!B202,"|",'Working Data'!C202,"|",'Working Data'!D202,"|",'Working Data'!E202,"|",'Working Data'!F202,"|",'Working Data'!G202,"|",'Working Data'!H202,"|",'Working Data'!I202,"|",'Working Data'!J202,"|",'Working Data'!K202,"|",'Working Data'!L202,"|",'Working Data'!M202)</f>
+        <v>_| |||||||||||</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" t="str">
+        <f>CONCATENATE('Working Data'!A203,"|",'Working Data'!B203,"|",'Working Data'!C203,"|",'Working Data'!D203,"|",'Working Data'!E203,"|",'Working Data'!F203,"|",'Working Data'!G203,"|",'Working Data'!H203,"|",'Working Data'!I203,"|",'Working Data'!J203,"|",'Working Data'!K203,"|",'Working Data'!L203,"|",'Working Data'!M203)</f>
+        <v>_| |||||||||||</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" t="str">
+        <f>CONCATENATE('Working Data'!A204,"|",'Working Data'!B204,"|",'Working Data'!C204,"|",'Working Data'!D204,"|",'Working Data'!E204,"|",'Working Data'!F204,"|",'Working Data'!G204,"|",'Working Data'!H204,"|",'Working Data'!I204,"|",'Working Data'!J204,"|",'Working Data'!K204,"|",'Working Data'!L204,"|",'Working Data'!M204)</f>
+        <v>||||||||||||</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" t="str">
+        <f>CONCATENATE('Working Data'!A205,"|",'Working Data'!B205,"|",'Working Data'!C205,"|",'Working Data'!D205,"|",'Working Data'!E205,"|",'Working Data'!F205,"|",'Working Data'!G205,"|",'Working Data'!H205,"|",'Working Data'!I205,"|",'Working Data'!J205,"|",'Working Data'!K205,"|",'Working Data'!L205,"|",'Working Data'!M205)</f>
+        <v>Mentos||||||||||||</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" t="str">
+        <f>CONCATENATE('Working Data'!A206,"|",'Working Data'!B206,"|",'Working Data'!C206,"|",'Working Data'!D206,"|",'Working Data'!E206,"|",'Working Data'!F206,"|",'Working Data'!G206,"|",'Working Data'!H206,"|",'Working Data'!I206,"|",'Working Data'!J206,"|",'Working Data'!K206,"|",'Working Data'!L206,"|",'Working Data'!M206)</f>
+        <v>||||||||||||</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" t="str">
+        <f>CONCATENATE('Working Data'!A207,"|",'Working Data'!B207,"|",'Working Data'!C207,"|",'Working Data'!D207,"|",'Working Data'!E207,"|",'Working Data'!F207,"|",'Working Data'!G207,"|",'Working Data'!H207,"|",'Working Data'!I207,"|",'Working Data'!J207,"|",'Working Data'!K207,"|",'Working Data'!L207,"|",'Working Data'!M207)</f>
+        <v>Cane'ls||||||||||||</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" t="str">
+        <f>CONCATENATE('Working Data'!A208,"|",'Working Data'!B208,"|",'Working Data'!C208,"|",'Working Data'!D208,"|",'Working Data'!E208,"|",'Working Data'!F208,"|",'Working Data'!G208,"|",'Working Data'!H208,"|",'Working Data'!I208,"|",'Working Data'!J208,"|",'Working Data'!K208,"|",'Working Data'!L208,"|",'Working Data'!M208)</f>
+        <v>quench||||||||||||</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" t="str">
+        <f>CONCATENATE('Working Data'!A209,"|",'Working Data'!B209,"|",'Working Data'!C209,"|",'Working Data'!D209,"|",'Working Data'!E209,"|",'Working Data'!F209,"|",'Working Data'!G209,"|",'Working Data'!H209,"|",'Working Data'!I209,"|",'Working Data'!J209,"|",'Working Data'!K209,"|",'Working Data'!L209,"|",'Working Data'!M209)</f>
+        <v>glee||||||||||||</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" t="str">
+        <f>CONCATENATE('Working Data'!A210,"|",'Working Data'!B210,"|",'Working Data'!C210,"|",'Working Data'!D210,"|",'Working Data'!E210,"|",'Working Data'!F210,"|",'Working Data'!G210,"|",'Working Data'!H210,"|",'Working Data'!I210,"|",'Working Data'!J210,"|",'Working Data'!K210,"|",'Working Data'!L210,"|",'Working Data'!M210)</f>
+        <v>blackjack||||||||||||</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" t="str">
+        <f>CONCATENATE('Working Data'!A211,"|",'Working Data'!B211,"|",'Working Data'!C211,"|",'Working Data'!D211,"|",'Working Data'!E211,"|",'Working Data'!F211,"|",'Working Data'!G211,"|",'Working Data'!H211,"|",'Working Data'!I211,"|",'Working Data'!J211,"|",'Working Data'!K211,"|",'Working Data'!L211,"|",'Working Data'!M211)</f>
+        <v>big league||||||||||||</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial seed gum images removed from lib folder and various text fixes
subscription page default (no shipments) and Chewlasticity description
change from flavor to size
</commit_message>
<xml_diff>
--- a/db/gums seed data v6.xlsx
+++ b/db/gums seed data v6.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="0" windowWidth="31700" windowHeight="19120" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4560" yWindow="0" windowWidth="31700" windowHeight="19120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Working Data" sheetId="1" r:id="rId1"/>
@@ -5452,8 +5452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P384"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A266" sqref="A266"/>
     </sheetView>
   </sheetViews>
@@ -18211,8 +18211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A327"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A251" workbookViewId="0">
-      <selection activeCell="A258" sqref="A258"/>
+    <sheetView showRuler="0" topLeftCell="A239" workbookViewId="0">
+      <selection sqref="A1:A267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>